<commit_message>
added sprint 1 pic
</commit_message>
<xml_diff>
--- a/Management Plan/Burndown Chart - Sprint 0.xlsx
+++ b/Management Plan/Burndown Chart - Sprint 0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CECS 491A\491Project\Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A364F-7E44-4505-A47D-030E6BA7D2FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA33DA93-438D-41B9-AC7C-E64A5287EDAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAC80B83-B7AF-4B17-A504-22BDF09CC802}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Day 0</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Day 15</t>
+  </si>
+  <si>
+    <t>Hours at the beginning of sprint of 0</t>
+  </si>
+  <si>
+    <t>Hours remaining</t>
   </si>
 </sst>
 </file>
@@ -166,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -174,11 +180,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -187,6 +255,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1667,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5ED47B-B067-447B-B835-A856D27FE495}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,6 +2321,28 @@
         <v>26</v>
       </c>
     </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K24" s="6">
+        <v>50</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K25" s="10">
+        <v>0</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added sprint 3 board
</commit_message>
<xml_diff>
--- a/Management Plan/Burndown Chart - Sprint 0.xlsx
+++ b/Management Plan/Burndown Chart - Sprint 0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CECS 491A\491Project\Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D0E1BC-CFAB-47C1-8545-D42F34F40CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BB3ADD-F4CB-4693-8B4F-9A6B5E69F73A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAC80B83-B7AF-4B17-A504-22BDF09CC802}"/>
   </bookViews>
@@ -128,7 +128,7 @@
     <t>Database</t>
   </si>
   <si>
-    <t>Hours at the beginning of sprint of 1</t>
+    <t>Hours at the beginning of sprint of 2</t>
   </si>
 </sst>
 </file>
@@ -447,10 +447,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>58</c:v>
@@ -459,40 +459,40 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,46 +599,46 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1748,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5ED47B-B067-447B-B835-A856D27FE495}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,43 +1828,43 @@
         <v>59</v>
       </c>
       <c r="F4">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G4">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I4">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="J4">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K4">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L4">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M4">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="N4">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="O4">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="P4">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="Q4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="R4">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2273,10 +2273,10 @@
         <v>15</v>
       </c>
       <c r="C18">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18">
         <v>58</v>
@@ -2285,40 +2285,40 @@
         <v>58</v>
       </c>
       <c r="G18">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H18">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I18">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="J18">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K18">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L18">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M18">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N18">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="O18">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="P18">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="Q18">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="R18">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2332,46 +2332,46 @@
         <v>59</v>
       </c>
       <c r="E19">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G19">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I19">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="J19">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K19">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L19">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M19">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="N19">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="O19">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="P19">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="Q19">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K25" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L25" s="11" t="s">
         <v>27</v>

</xml_diff>